<commit_message>
added capital costs for petrol and lpg buses
</commit_message>
<xml_diff>
--- a/PREPARE-TIMES-NZ/data_raw/eeca_data/tcoe/vehicle_costs_2023.xlsx
+++ b/PREPARE-TIMES-NZ/data_raw/eeca_data/tcoe/vehicle_costs_2023.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\weerasa\git\TIMES-NZ-Model-Files\PREPARE-TIMES-NZ\data_raw\eeca_data\tcoe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FFCD24-E628-4760-ADC8-D5E33DC7D0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ECA11C-728A-4564-B8B6-7FE190E4E1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11928" yWindow="-17280" windowWidth="20832" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7890" yWindow="-14510" windowWidth="34620" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AG_costs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AG_costs!$A$1:$K$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AG_costs!$A$1:$K$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="102">
   <si>
     <t>Vehicle</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>Assumed same as Diesel ICE</t>
+  </si>
+  <si>
+    <t>LPG</t>
   </si>
 </sst>
 </file>
@@ -366,7 +372,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,13 +383,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,14 +415,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -721,28 +717,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +770,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -811,7 +807,7 @@
         <v>0.10814285714285714</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -848,7 +844,7 @@
         <v>9.0040000000000009E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -885,7 +881,7 @@
         <v>9.4412380952380942E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -922,7 +918,7 @@
         <v>9.0998095238095239E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -959,7 +955,7 @@
         <v>7.4216190476190477E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1002,7 +998,7 @@
         <v>42000</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1039,7 +1035,7 @@
         <v>6.4015238095238097E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1079,7 +1075,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1119,7 +1115,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1150,7 +1146,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1190,7 +1186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1227,7 +1223,7 @@
         <v>5.8269523809523813E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1264,7 +1260,7 @@
         <v>8.0716190476190469E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1301,7 +1297,7 @@
         <v>9.4412380952380942E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1338,7 +1334,7 @@
         <v>9.3452380952380953E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1375,7 +1371,7 @@
         <v>0.10921428571428571</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1412,7 +1408,7 @@
         <v>5.1729523809523809E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1449,7 +1445,7 @@
         <v>4.5491428571428572E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1486,7 +1482,7 @@
         <v>5.4160000000000007E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1523,7 +1519,7 @@
         <v>7.7777142857142864E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1560,7 +1556,7 @@
         <v>9.7861904761904761E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1597,7 +1593,7 @@
         <v>7.1547619047619054E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1634,7 +1630,7 @@
         <v>7.8446666666666678E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1671,7 +1667,7 @@
         <v>4.9151428571428575E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1708,7 +1704,7 @@
         <v>4.6290476190476194E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1745,7 +1741,7 @@
         <v>7.298857142857143E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1782,7 +1778,7 @@
         <v>6.3365714285714289E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1819,7 +1815,7 @@
         <v>8.3500000000000005E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -1856,7 +1852,7 @@
         <v>8.3071428571428574E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1893,7 +1889,7 @@
         <v>0.10702380952380952</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1930,7 +1926,7 @@
         <v>3.5460000000000005E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -1967,7 +1963,7 @@
         <v>5.4425714285714286E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -2004,7 +2000,7 @@
         <v>5.4417142857142858E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -2029,7 +2025,7 @@
       <c r="H35" s="2"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2054,7 +2050,7 @@
       <c r="H36" s="2"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2079,7 +2075,7 @@
       <c r="H37" s="2"/>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2104,7 +2100,7 @@
       <c r="H38" s="2"/>
       <c r="K38" s="3"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -2129,7 +2125,7 @@
       <c r="H39" s="2"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -2154,7 +2150,7 @@
       <c r="H40" s="2"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -2179,7 +2175,7 @@
       <c r="H41" s="2"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>95</v>
       </c>
@@ -2204,7 +2200,7 @@
       <c r="H42" s="2"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2229,7 +2225,7 @@
       <c r="H43" s="2"/>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -2254,7 +2250,7 @@
       <c r="H44" s="2"/>
       <c r="K44" s="3"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -2279,7 +2275,7 @@
       <c r="H45" s="2"/>
       <c r="K45" s="3"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>64</v>
       </c>
@@ -2304,7 +2300,7 @@
       <c r="H46" s="2"/>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -2329,7 +2325,7 @@
       <c r="H47" s="2"/>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -2354,7 +2350,7 @@
       <c r="H48" s="2"/>
       <c r="K48" s="3"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -2378,7 +2374,7 @@
       </c>
       <c r="K49" s="3"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -2403,7 +2399,7 @@
       </c>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -2427,7 +2423,7 @@
       </c>
       <c r="K51" s="3"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -2451,7 +2447,7 @@
       </c>
       <c r="K52" s="3"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -2475,7 +2471,7 @@
       </c>
       <c r="K53" s="3"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -2501,7 +2497,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -2527,7 +2523,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>75</v>
       </c>
@@ -2553,7 +2549,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -2577,7 +2573,7 @@
       </c>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -2601,7 +2597,7 @@
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -2625,7 +2621,7 @@
       </c>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>99</v>
       </c>
@@ -2648,11 +2644,54 @@
         <v>454410</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G61" s="4"/>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61">
+        <v>2025</v>
+      </c>
+      <c r="D61" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" t="s">
+        <v>60</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61">
+        <v>400000</v>
+      </c>
+      <c r="K61" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62">
+        <v>2025</v>
+      </c>
+      <c r="D62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" t="s">
+        <v>60</v>
+      </c>
+      <c r="F62" t="s">
+        <v>101</v>
+      </c>
+      <c r="G62">
+        <v>400000</v>
+      </c>
+      <c r="K62" s="3">
+        <v>0.86</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K59" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K63" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D58" xr:uid="{6A948511-6061-484C-8C56-4360A77F9759}">
       <formula1>$O$7:$O$12</formula1>

</xml_diff>

<commit_message>
added capital costs for petrol and lpg buses (#174)
* added capital costs for petrol and lpg buses

* add industrial waste water supply into municipal solid waste and waste water category
</commit_message>
<xml_diff>
--- a/PREPARE-TIMES-NZ/data_raw/eeca_data/tcoe/vehicle_costs_2023.xlsx
+++ b/PREPARE-TIMES-NZ/data_raw/eeca_data/tcoe/vehicle_costs_2023.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\weerasa\git\TIMES-NZ-Model-Files\PREPARE-TIMES-NZ\data_raw\eeca_data\tcoe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FFCD24-E628-4760-ADC8-D5E33DC7D0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ECA11C-728A-4564-B8B6-7FE190E4E1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11928" yWindow="-17280" windowWidth="20832" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7890" yWindow="-14510" windowWidth="34620" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AG_costs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AG_costs!$A$1:$K$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AG_costs!$A$1:$K$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="102">
   <si>
     <t>Vehicle</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>Assumed same as Diesel ICE</t>
+  </si>
+  <si>
+    <t>LPG</t>
   </si>
 </sst>
 </file>
@@ -366,7 +372,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,13 +383,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,14 +415,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -721,28 +717,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +770,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -811,7 +807,7 @@
         <v>0.10814285714285714</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -848,7 +844,7 @@
         <v>9.0040000000000009E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -885,7 +881,7 @@
         <v>9.4412380952380942E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -922,7 +918,7 @@
         <v>9.0998095238095239E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -959,7 +955,7 @@
         <v>7.4216190476190477E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1002,7 +998,7 @@
         <v>42000</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1039,7 +1035,7 @@
         <v>6.4015238095238097E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1079,7 +1075,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1119,7 +1115,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1150,7 +1146,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1190,7 +1186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1227,7 +1223,7 @@
         <v>5.8269523809523813E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1264,7 +1260,7 @@
         <v>8.0716190476190469E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1301,7 +1297,7 @@
         <v>9.4412380952380942E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1338,7 +1334,7 @@
         <v>9.3452380952380953E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1375,7 +1371,7 @@
         <v>0.10921428571428571</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1412,7 +1408,7 @@
         <v>5.1729523809523809E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1449,7 +1445,7 @@
         <v>4.5491428571428572E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1486,7 +1482,7 @@
         <v>5.4160000000000007E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1523,7 +1519,7 @@
         <v>7.7777142857142864E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1560,7 +1556,7 @@
         <v>9.7861904761904761E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1597,7 +1593,7 @@
         <v>7.1547619047619054E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1634,7 +1630,7 @@
         <v>7.8446666666666678E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1671,7 +1667,7 @@
         <v>4.9151428571428575E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1708,7 +1704,7 @@
         <v>4.6290476190476194E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1745,7 +1741,7 @@
         <v>7.298857142857143E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1782,7 +1778,7 @@
         <v>6.3365714285714289E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1819,7 +1815,7 @@
         <v>8.3500000000000005E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -1856,7 +1852,7 @@
         <v>8.3071428571428574E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1893,7 +1889,7 @@
         <v>0.10702380952380952</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1930,7 +1926,7 @@
         <v>3.5460000000000005E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -1967,7 +1963,7 @@
         <v>5.4425714285714286E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -2004,7 +2000,7 @@
         <v>5.4417142857142858E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -2029,7 +2025,7 @@
       <c r="H35" s="2"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2054,7 +2050,7 @@
       <c r="H36" s="2"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2079,7 +2075,7 @@
       <c r="H37" s="2"/>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2104,7 +2100,7 @@
       <c r="H38" s="2"/>
       <c r="K38" s="3"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -2129,7 +2125,7 @@
       <c r="H39" s="2"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -2154,7 +2150,7 @@
       <c r="H40" s="2"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -2179,7 +2175,7 @@
       <c r="H41" s="2"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>95</v>
       </c>
@@ -2204,7 +2200,7 @@
       <c r="H42" s="2"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2229,7 +2225,7 @@
       <c r="H43" s="2"/>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -2254,7 +2250,7 @@
       <c r="H44" s="2"/>
       <c r="K44" s="3"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -2279,7 +2275,7 @@
       <c r="H45" s="2"/>
       <c r="K45" s="3"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>64</v>
       </c>
@@ -2304,7 +2300,7 @@
       <c r="H46" s="2"/>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -2329,7 +2325,7 @@
       <c r="H47" s="2"/>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -2354,7 +2350,7 @@
       <c r="H48" s="2"/>
       <c r="K48" s="3"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -2378,7 +2374,7 @@
       </c>
       <c r="K49" s="3"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -2403,7 +2399,7 @@
       </c>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -2427,7 +2423,7 @@
       </c>
       <c r="K51" s="3"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -2451,7 +2447,7 @@
       </c>
       <c r="K52" s="3"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -2475,7 +2471,7 @@
       </c>
       <c r="K53" s="3"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -2501,7 +2497,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -2527,7 +2523,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>75</v>
       </c>
@@ -2553,7 +2549,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -2577,7 +2573,7 @@
       </c>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -2601,7 +2597,7 @@
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -2625,7 +2621,7 @@
       </c>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>99</v>
       </c>
@@ -2648,11 +2644,54 @@
         <v>454410</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G61" s="4"/>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61">
+        <v>2025</v>
+      </c>
+      <c r="D61" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" t="s">
+        <v>60</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61">
+        <v>400000</v>
+      </c>
+      <c r="K61" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62">
+        <v>2025</v>
+      </c>
+      <c r="D62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" t="s">
+        <v>60</v>
+      </c>
+      <c r="F62" t="s">
+        <v>101</v>
+      </c>
+      <c r="G62">
+        <v>400000</v>
+      </c>
+      <c r="K62" s="3">
+        <v>0.86</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K59" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K63" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D58" xr:uid="{6A948511-6061-484C-8C56-4360A77F9759}">
       <formula1>$O$7:$O$12</formula1>

</xml_diff>